<commit_message>
Identificando o usuário do PC
</commit_message>
<xml_diff>
--- a/Files/output/Necessidade - Slitter.xlsx
+++ b/Files/output/Necessidade - Slitter.xlsx
@@ -20,16 +20,13 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -438,57 +426,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Ordem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Texto breve material</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Espessura Padrão (mm)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Matriz de Conformação</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Data sequenciamento</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Qtd.necessária (EINHEIT)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Utilização livre</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Demanda Acumulada</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Saldo Projetado</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -516,7 +504,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G2" t="n">
@@ -559,7 +547,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G3" t="n">
@@ -602,7 +590,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G4" t="n">
@@ -645,7 +633,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G5" t="n">
@@ -688,7 +676,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G6" t="n">
@@ -731,7 +719,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G7" t="n">
@@ -774,7 +762,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G8" t="n">
@@ -817,7 +805,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G9" t="n">
@@ -860,7 +848,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G10" t="n">
@@ -903,7 +891,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G11" t="n">
@@ -946,7 +934,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G12" t="n">
@@ -989,7 +977,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G13" t="n">
@@ -1032,7 +1020,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G14" t="n">
@@ -1075,7 +1063,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G15" t="n">
@@ -1118,7 +1106,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G16" t="n">
@@ -1161,7 +1149,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G17" t="n">
@@ -1204,7 +1192,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G18" t="n">
@@ -1247,7 +1235,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G19" t="n">
@@ -1290,7 +1278,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="1" t="n">
         <v>46066</v>
       </c>
       <c r="G20" t="n">
@@ -1333,7 +1321,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="1" t="n">
         <v>46067</v>
       </c>
       <c r="G21" t="n">
@@ -1376,7 +1364,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="1" t="n">
         <v>46070</v>
       </c>
       <c r="G22" t="n">
@@ -1419,7 +1407,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G23" t="n">
@@ -1462,7 +1450,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G24" t="n">
@@ -1505,7 +1493,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G25" t="n">
@@ -1548,7 +1536,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G26" t="n">
@@ -1591,7 +1579,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G27" t="n">
@@ -1634,7 +1622,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G28" t="n">
@@ -1677,7 +1665,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="1" t="n">
         <v>46071</v>
       </c>
       <c r="G29" t="n">
@@ -1720,7 +1708,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G30" t="n">
@@ -1763,7 +1751,7 @@
           <t>60,30-2"PT</t>
         </is>
       </c>
-      <c r="F31" s="2" t="n">
+      <c r="F31" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G31" t="n">
@@ -1806,7 +1794,7 @@
           <t>60,30-2"PT</t>
         </is>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F32" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G32" t="n">
@@ -1849,7 +1837,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F33" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G33" t="n">
@@ -1892,7 +1880,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F34" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G34" t="n">
@@ -1935,7 +1923,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="F35" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G35" t="n">
@@ -1978,7 +1966,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G36" t="n">
@@ -2021,7 +2009,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G37" t="n">
@@ -2064,7 +2052,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F38" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G38" t="n">
@@ -2107,7 +2095,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F39" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G39" t="n">
@@ -2150,7 +2138,7 @@
           <t>63,50-2.1/2"</t>
         </is>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F40" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G40" t="n">
@@ -2193,7 +2181,7 @@
           <t>60,30-2"PT</t>
         </is>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="F41" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G41" t="n">
@@ -2236,7 +2224,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F42" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G42" t="n">
@@ -2279,7 +2267,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F43" s="2" t="n">
+      <c r="F43" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G43" t="n">
@@ -2322,7 +2310,7 @@
           <t>60,30-2"PT</t>
         </is>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G44" t="n">
@@ -2365,7 +2353,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F45" s="2" t="n">
+      <c r="F45" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G45" t="n">
@@ -2408,7 +2396,7 @@
           <t>19,05-3/4"</t>
         </is>
       </c>
-      <c r="F46" s="2" t="n">
+      <c r="F46" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G46" t="n">
@@ -2451,7 +2439,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F47" s="2" t="n">
+      <c r="F47" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G47" t="n">
@@ -2494,7 +2482,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F48" s="2" t="n">
+      <c r="F48" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G48" t="n">
@@ -2537,7 +2525,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F49" s="2" t="n">
+      <c r="F49" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G49" t="n">
@@ -2580,7 +2568,7 @@
           <t>60,30-2"PT</t>
         </is>
       </c>
-      <c r="F50" s="2" t="n">
+      <c r="F50" s="1" t="n">
         <v>46072</v>
       </c>
       <c r="G50" t="n">
@@ -2623,7 +2611,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F51" s="2" t="n">
+      <c r="F51" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G51" t="n">
@@ -2666,7 +2654,7 @@
           <t>63,50-2.1/2"</t>
         </is>
       </c>
-      <c r="F52" s="2" t="n">
+      <c r="F52" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G52" t="n">
@@ -2709,7 +2697,7 @@
           <t>63,50-2.1/2"</t>
         </is>
       </c>
-      <c r="F53" s="2" t="n">
+      <c r="F53" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G53" t="n">
@@ -2752,7 +2740,7 @@
           <t>63,50-2.1/2"</t>
         </is>
       </c>
-      <c r="F54" s="2" t="n">
+      <c r="F54" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G54" t="n">
@@ -2795,7 +2783,7 @@
           <t>63,50-2.1/2"</t>
         </is>
       </c>
-      <c r="F55" s="2" t="n">
+      <c r="F55" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G55" t="n">
@@ -2838,7 +2826,7 @@
           <t>47,62-1.7/8"</t>
         </is>
       </c>
-      <c r="F56" s="2" t="n">
+      <c r="F56" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G56" t="n">
@@ -2881,7 +2869,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G57" t="n">
@@ -2924,7 +2912,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F58" s="2" t="n">
+      <c r="F58" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G58" t="n">
@@ -2967,7 +2955,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F59" s="2" t="n">
+      <c r="F59" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G59" t="n">
@@ -3010,7 +2998,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G60" t="n">
@@ -3053,7 +3041,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F61" s="2" t="n">
+      <c r="F61" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G61" t="n">
@@ -3096,7 +3084,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F62" s="2" t="n">
+      <c r="F62" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G62" t="n">
@@ -3139,7 +3127,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G63" t="n">
@@ -3182,7 +3170,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F64" s="2" t="n">
+      <c r="F64" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G64" t="n">
@@ -3225,7 +3213,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F65" s="2" t="n">
+      <c r="F65" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G65" t="n">
@@ -3268,7 +3256,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G66" t="n">
@@ -3311,7 +3299,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F67" s="2" t="n">
+      <c r="F67" s="1" t="n">
         <v>46073</v>
       </c>
       <c r="G67" t="n">
@@ -3354,7 +3342,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F68" s="2" t="n">
+      <c r="F68" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G68" t="n">
@@ -3397,7 +3385,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F69" s="2" t="n">
+      <c r="F69" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G69" t="n">
@@ -3440,7 +3428,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F70" s="2" t="n">
+      <c r="F70" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G70" t="n">
@@ -3483,7 +3471,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F71" s="2" t="n">
+      <c r="F71" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G71" t="n">
@@ -3526,7 +3514,7 @@
           <t>22,22-7/8"</t>
         </is>
       </c>
-      <c r="F72" s="2" t="n">
+      <c r="F72" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G72" t="n">
@@ -3569,7 +3557,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F73" s="2" t="n">
+      <c r="F73" s="1" t="n">
         <v>46074</v>
       </c>
       <c r="G73" t="n">
@@ -3612,7 +3600,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F74" s="2" t="n">
+      <c r="F74" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G74" t="n">
@@ -3655,7 +3643,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F75" s="2" t="n">
+      <c r="F75" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G75" t="n">
@@ -3698,7 +3686,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F76" s="2" t="n">
+      <c r="F76" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G76" t="n">
@@ -3741,7 +3729,7 @@
           <t>50,80-2"</t>
         </is>
       </c>
-      <c r="F77" s="2" t="n">
+      <c r="F77" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G77" t="n">
@@ -3784,7 +3772,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F78" s="2" t="n">
+      <c r="F78" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G78" t="n">
@@ -3827,7 +3815,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F79" s="2" t="n">
+      <c r="F79" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G79" t="n">
@@ -3870,7 +3858,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F80" s="2" t="n">
+      <c r="F80" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G80" t="n">
@@ -3913,7 +3901,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F81" s="2" t="n">
+      <c r="F81" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G81" t="n">
@@ -3956,7 +3944,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F82" s="2" t="n">
+      <c r="F82" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G82" t="n">
@@ -3999,7 +3987,7 @@
           <t>101,60-4"</t>
         </is>
       </c>
-      <c r="F83" s="2" t="n">
+      <c r="F83" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G83" t="n">
@@ -4042,7 +4030,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F84" s="2" t="n">
+      <c r="F84" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G84" t="n">
@@ -4085,7 +4073,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F85" s="2" t="n">
+      <c r="F85" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G85" t="n">
@@ -4128,7 +4116,7 @@
           <t>26,70-3/4"PT</t>
         </is>
       </c>
-      <c r="F86" s="2" t="n">
+      <c r="F86" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G86" t="n">
@@ -4171,7 +4159,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F87" s="2" t="n">
+      <c r="F87" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G87" t="n">
@@ -4214,7 +4202,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F88" s="2" t="n">
+      <c r="F88" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G88" t="n">
@@ -4257,7 +4245,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F89" s="2" t="n">
+      <c r="F89" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G89" t="n">
@@ -4300,7 +4288,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F90" s="2" t="n">
+      <c r="F90" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G90" t="n">
@@ -4343,7 +4331,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F91" s="2" t="n">
+      <c r="F91" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G91" t="n">
@@ -4386,7 +4374,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F92" s="2" t="n">
+      <c r="F92" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G92" t="n">
@@ -4429,7 +4417,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F93" s="2" t="n">
+      <c r="F93" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G93" t="n">
@@ -4472,7 +4460,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F94" s="2" t="n">
+      <c r="F94" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G94" t="n">
@@ -4515,7 +4503,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F95" s="2" t="n">
+      <c r="F95" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G95" t="n">
@@ -4558,7 +4546,7 @@
           <t>76,20-3"</t>
         </is>
       </c>
-      <c r="F96" s="2" t="n">
+      <c r="F96" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G96" t="n">
@@ -4601,7 +4589,7 @@
           <t>15,87-5/8"</t>
         </is>
       </c>
-      <c r="F97" s="2" t="n">
+      <c r="F97" s="1" t="n">
         <v>46076</v>
       </c>
       <c r="G97" t="n">
@@ -4644,7 +4632,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F98" s="2" t="n">
+      <c r="F98" s="1" t="n">
         <v>46077</v>
       </c>
       <c r="G98" t="n">
@@ -4687,7 +4675,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F99" s="2" t="n">
+      <c r="F99" s="1" t="n">
         <v>46077</v>
       </c>
       <c r="G99" t="n">
@@ -4730,7 +4718,7 @@
           <t>31,75-1.1/4"</t>
         </is>
       </c>
-      <c r="F100" s="2" t="n">
+      <c r="F100" s="1" t="n">
         <v>46077</v>
       </c>
       <c r="G100" t="n">
@@ -4773,7 +4761,7 @@
           <t>21,30-1/2"PT</t>
         </is>
       </c>
-      <c r="F101" s="2" t="n">
+      <c r="F101" s="1" t="n">
         <v>46078</v>
       </c>
       <c r="G101" t="n">
@@ -4816,7 +4804,7 @@
           <t>21,30-1/2"PT</t>
         </is>
       </c>
-      <c r="F102" s="2" t="n">
+      <c r="F102" s="1" t="n">
         <v>46080</v>
       </c>
       <c r="G102" t="n">
@@ -4859,7 +4847,7 @@
           <t>21,30-1/2"PT</t>
         </is>
       </c>
-      <c r="F103" s="2" t="n">
+      <c r="F103" s="1" t="n">
         <v>46080</v>
       </c>
       <c r="G103" t="n">
@@ -4902,7 +4890,7 @@
           <t>25,40-1"</t>
         </is>
       </c>
-      <c r="F104" s="2" t="n">
+      <c r="F104" s="1" t="n">
         <v>46086</v>
       </c>
       <c r="G104" t="n">

</xml_diff>